<commit_message>
fixed cbm calculations 😐 + various changes
- renamed package to yandiyacbm
- had to rename all instances of package being imported
- also found out that the value used in the cbm calculations was out by a factor of 1000 this was because I though product details was in cm when it in fact in mm 😐
- This fixes issue #14 , which I though was already fixed 😐
</commit_message>
<xml_diff>
--- a/main/database/pallet-db.xlsx
+++ b/main/database/pallet-db.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -399,9 +399,6 @@
       <c r="F1" t="str">
         <v>maxWeight</v>
       </c>
-      <c r="G1" t="str">
-        <v>price</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -422,9 +419,6 @@
       <c r="F2" t="str">
         <v>300</v>
       </c>
-      <c r="G2" t="str">
-        <v>32</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -445,9 +439,6 @@
       <c r="F3" t="str">
         <v>600</v>
       </c>
-      <c r="G3" t="str">
-        <v>33</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -468,9 +459,6 @@
       <c r="F4" t="str">
         <v>1200</v>
       </c>
-      <c r="G4" t="str">
-        <v>35.50</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -491,9 +479,6 @@
       <c r="F5" t="str">
         <v>300</v>
       </c>
-      <c r="G5" t="str">
-        <v>31</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -514,9 +499,6 @@
       <c r="F6" t="str">
         <v>600</v>
       </c>
-      <c r="G6" t="str">
-        <v>31</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -537,13 +519,10 @@
       <c r="F7" t="str">
         <v>1200</v>
       </c>
-      <c r="G7" t="str">
-        <v>33</v>
-      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>